<commit_message>
Signup Page Completed 29-04-2024
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAED\src\resources\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -69,12 +69,55 @@
   </si>
   <si>
     <t>aditya689@yopmail.com</t>
+  </si>
+  <si>
+    <t>aditya327@yopmail.com</t>
+  </si>
+  <si>
+    <t>aditya549@noreply.fr</t>
+  </si>
+  <si>
+    <t>adityab259@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityec914@yopmail.com</t>
+  </si>
+  <si>
+    <t>aditygd151@yopmail.com</t>
+  </si>
+  <si>
+    <t>aditycb973@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityaa468@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityge868@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityac769@yopmail.com</t>
+  </si>
+  <si>
+    <t>aditygf387@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityga955@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityed167@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityde783@yopmail.com</t>
+  </si>
+  <si>
+    <t>adityag363@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,8 +448,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
-    <col min="3" max="3" width="52" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="58.28515625"/>
+    <col min="3" max="3" customWidth="true" width="52.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,74 +523,74 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="14">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="15">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="16">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="17">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="18">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="19">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="20">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="21">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="22">
+      <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="23">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="24">
+      <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="25">
+      <c r="B25" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Signup Page Completed 10-05-2024
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAED\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Project details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -111,13 +112,15 @@
   </si>
   <si>
     <t>adityag363@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Name </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,14 +445,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C428"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="58.28515625"/>
-    <col min="3" max="3" customWidth="true" width="52.0"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,97 +526,97 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2604,4 +2607,28 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Signup Page Completed 21-05-2024
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAED\src\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -115,12 +115,52 @@
   </si>
   <si>
     <t xml:space="preserve">Project Name </t>
+  </si>
+  <si>
+    <t>Solar Project CD</t>
+  </si>
+  <si>
+    <t>Solar Project CB</t>
+  </si>
+  <si>
+    <t>Solar Project BC</t>
+  </si>
+  <si>
+    <t>Solar Project AA</t>
+  </si>
+  <si>
+    <t>Solar Project BB</t>
+  </si>
+  <si>
+    <t>Solar Project DC</t>
+  </si>
+  <si>
+    <t>Solar Project DA</t>
+  </si>
+  <si>
+    <t>Solar Project BA</t>
+  </si>
+  <si>
+    <t>Solar Project CA</t>
+  </si>
+  <si>
+    <t>Solar Project DD</t>
+  </si>
+  <si>
+    <t>Solar Project AB</t>
+  </si>
+  <si>
+    <t>Solar Project AC</t>
+  </si>
+  <si>
+    <t>Solar Project BD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,8 +491,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
-    <col min="3" max="3" width="52" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="58.28515625"/>
+    <col min="3" max="3" customWidth="true" width="52.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2611,7 +2651,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -2619,8 +2659,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="21.5703125"/>
+    <col min="2" max="2" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2628,6 +2668,196 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commited signup, login, homepage completed 04-09-2024
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Solar Project BD</t>
+  </si>
+  <si>
+    <t>Solar Project AD</t>
+  </si>
+  <si>
+    <t>Solar Project CC</t>
+  </si>
+  <si>
+    <t>Solar Project DB</t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -2858,6 +2867,141 @@
         <v>41</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
login signup and buyandsell running code
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Solar Project BD</t>
+  </si>
+  <si>
+    <t>Solar Project DB</t>
+  </si>
+  <si>
+    <t>Solar Project AD</t>
+  </si>
+  <si>
+    <t>Solar Project CC</t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -2858,6 +2867,126 @@
         <v>41</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed the issue for the scripts
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -2987,6 +2987,21 @@
         <v>31</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Running chrome in non headless mode
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:A67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3002,6 +3002,11 @@
         <v>39</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the Buy and sell project flow admin accept flow
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A67"/>
+  <dimension ref="A1:A98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3007,6 +3007,161 @@
         <v>34</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Set all the file and testng.xml
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A98"/>
+  <dimension ref="A1:A102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3162,6 +3162,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
setup devTools for the OTP
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A111"/>
+  <dimension ref="A1:A113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3227,6 +3227,16 @@
         <v>44</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
setep devTool and testng xml and the container
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A113"/>
+  <dimension ref="A1:A124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3237,6 +3237,61 @@
         <v>41</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update the gitlab file
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -2660,7 +2660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A129"/>
+  <dimension ref="A1:A131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3317,6 +3317,16 @@
         <v>31</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
buy and sell flow added
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="51">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>Solar Project CC</t>
+  </si>
+  <si>
+    <t>Solar Project CFB</t>
+  </si>
+  <si>
+    <t>Solar Project FGF</t>
+  </si>
+  <si>
+    <t>Solar Project HHE</t>
+  </si>
+  <si>
+    <t>Solar Project HBB</t>
+  </si>
+  <si>
+    <t>Solar Project AIB</t>
   </si>
 </sst>
 </file>
@@ -498,13 +513,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="58.28515625"/>
+    <col min="2" max="2" customWidth="true" width="58.33203125"/>
     <col min="3" max="3" customWidth="true" width="52.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,2137 +530,2137 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>415</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>416</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>417</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>418</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>419</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>420</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>421</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>422</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>423</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>424</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>425</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>426</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>427</v>
       </c>
@@ -2660,671 +2675,736 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A131"/>
+  <dimension ref="A1:A144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125"/>
+    <col min="1" max="1" customWidth="true" width="21.5546875"/>
     <col min="2" max="2" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
site visit schedule completed
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Solar Project ADA</t>
+  </si>
+  <si>
+    <t>Solar Project AHA</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2684,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A146"/>
+  <dimension ref="A1:A147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
@@ -3423,6 +3426,11 @@
         <v>52</v>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
buy an sell complete
</commit_message>
<xml_diff>
--- a/src/resources/Consumer_signup_ids.xlsx
+++ b/src/resources/Consumer_signup_ids.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
   <si>
     <t xml:space="preserve">SR no </t>
   </si>
@@ -156,13 +156,82 @@
     <t>Solar Project BD</t>
   </si>
   <si>
+    <t>Solar Project DB</t>
+  </si>
+  <si>
     <t>Solar Project AD</t>
   </si>
   <si>
     <t>Solar Project CC</t>
   </si>
   <si>
-    <t>Solar Project DB</t>
+    <t>Solar Project CFB</t>
+  </si>
+  <si>
+    <t>Solar Project FGF</t>
+  </si>
+  <si>
+    <t>Solar Project HHE</t>
+  </si>
+  <si>
+    <t>Solar Project HBB</t>
+  </si>
+  <si>
+    <t>Solar Project AIB</t>
+  </si>
+  <si>
+    <t>Solar Project GDI</t>
+  </si>
+  <si>
+    <t>Solar Project ADA</t>
+  </si>
+  <si>
+    <t>Solar Project AHA</t>
+  </si>
+  <si>
+    <t>Solar Project GHC</t>
+  </si>
+  <si>
+    <t>Solar Project IIG</t>
+  </si>
+  <si>
+    <t>Solar Project IIH</t>
+  </si>
+  <si>
+    <t>Solar Project IFB</t>
+  </si>
+  <si>
+    <t>Solar Project DHA</t>
+  </si>
+  <si>
+    <t>Solar Project BCG</t>
+  </si>
+  <si>
+    <t>Solar Project CIC</t>
+  </si>
+  <si>
+    <t>Solar Project BEB</t>
+  </si>
+  <si>
+    <t>Solar Project GHH</t>
+  </si>
+  <si>
+    <t>Solar Project IAB</t>
+  </si>
+  <si>
+    <t>Solar Project CHE</t>
+  </si>
+  <si>
+    <t>Solar Project HGF</t>
+  </si>
+  <si>
+    <t>Solar Project EHG</t>
+  </si>
+  <si>
+    <t>Solar Project DBB</t>
+  </si>
+  <si>
+    <t>Solar Project GAD</t>
   </si>
 </sst>
 </file>
@@ -498,13 +567,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="58.28515625"/>
+    <col min="2" max="2" customWidth="true" width="58.33203125"/>
     <col min="3" max="3" customWidth="true" width="52.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,2137 +584,2137 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>415</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>416</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>417</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>418</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>419</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>420</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>421</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>422</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>423</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>424</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>425</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>426</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>427</v>
       </c>
@@ -2660,346 +2729,831 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:A163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.5703125"/>
+    <col min="1" max="1" customWidth="true" width="21.5546875"/>
     <col min="2" max="2" customWidth="true" width="24.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>32</v>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>